<commit_message>
Upload updated evaporation file with line 15 in sheet from_resources_values corrected
</commit_message>
<xml_diff>
--- a/qa/evaporation.xlsx
+++ b/qa/evaporation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/barr_colleen_epa_gov/Documents/Profile/Documents/SWMM-CAT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbarr02\OneDrive - Environmental Protection Agency (EPA)\Profile\Desktop\GitHub\Data-Processing-for-SWC-and-SWMM-CAT\qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{EC6548AB-38E8-459C-8096-723A39A41D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0CFAE6-C3A3-4427-AC18-B8B8DC360A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="my_calc_changes" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,23 @@
     <sheet name="comparison_changes" sheetId="4" r:id="rId5"/>
     <sheet name="comparison_monthly_evap" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="20">
   <si>
     <t>TEMP2035HotDry</t>
   </si>
@@ -90,7 +101,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -568,8 +579,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -924,7 +936,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3621,11 +3633,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4291,43 +4303,43 @@
         <v>1</v>
       </c>
       <c r="C15">
-        <v>3.9E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="D15">
-        <v>5.3999999999999999E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="E15">
-        <v>0.09</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="F15">
-        <v>0.129</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="G15">
-        <v>0.17399999999999999</v>
+        <v>0.14099999999999999</v>
       </c>
       <c r="H15">
-        <v>0.23</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="I15">
-        <v>0.25</v>
+        <v>0.184</v>
       </c>
       <c r="J15">
-        <v>0.216</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="K15">
-        <v>0.16500000000000001</v>
+        <v>0.111</v>
       </c>
       <c r="L15">
-        <v>0.1</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="M15">
-        <v>5.6000000000000001E-2</v>
+        <v>0.03</v>
       </c>
       <c r="N15">
-        <v>3.5999999999999997E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="O15">
-        <v>46.984999999999999</v>
+        <v>33.631</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
@@ -6499,7 +6511,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6995,7 +7007,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7522,11 +7534,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8301,60 +8313,60 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15">
+    <row r="15" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
         <v>72793524234</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <f>from_resources_values!C15 - my_calc_changes!C15 - my_monthly_evap!C$4</f>
-        <v>1.6E-2</v>
-      </c>
-      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
         <f>from_resources_values!D15 - my_calc_changes!D15 - my_monthly_evap!D$4</f>
-        <v>1.6E-2</v>
-      </c>
-      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
         <f>from_resources_values!E15 - my_calc_changes!E15 - my_monthly_evap!E$4</f>
-        <v>2.3999999999999994E-2</v>
-      </c>
-      <c r="F15">
+        <v>1.0000000000000009E-3</v>
+      </c>
+      <c r="F15" s="1">
         <f>from_resources_values!F15 - my_calc_changes!F15 - my_monthly_evap!F$4</f>
-        <v>2.7999999999999997E-2</v>
-      </c>
-      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
         <f>from_resources_values!G15 - my_calc_changes!G15 - my_monthly_evap!G$4</f>
-        <v>3.2999999999999974E-2</v>
-      </c>
-      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
         <f>from_resources_values!H15 - my_calc_changes!H15 - my_monthly_evap!H$4</f>
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="I15">
+        <v>-1.0000000000000009E-3</v>
+      </c>
+      <c r="I15" s="1">
         <f>from_resources_values!I15 - my_calc_changes!I15 - my_monthly_evap!I$4</f>
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
         <f>from_resources_values!J15 - my_calc_changes!J15 - my_monthly_evap!J$4</f>
-        <v>5.1999999999999991E-2</v>
-      </c>
-      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
         <f>from_resources_values!K15 - my_calc_changes!K15 - my_monthly_evap!K$4</f>
-        <v>5.3000000000000005E-2</v>
-      </c>
-      <c r="L15">
+        <v>-1.0000000000000009E-3</v>
+      </c>
+      <c r="L15" s="1">
         <f>from_resources_values!L15 - my_calc_changes!L15 - my_monthly_evap!L$4</f>
-        <v>4.1000000000000002E-2</v>
-      </c>
-      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
         <f>from_resources_values!M15 - my_calc_changes!M15 - my_monthly_evap!M$4</f>
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="N15" s="1">
         <f>from_resources_values!N15 - my_calc_changes!N15 - my_monthly_evap!N$4</f>
-        <v>1.6999999999999998E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
@@ -10939,7 +10951,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>